<commit_message>
Fixed import of report and fixed context id error
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.0.xlsx
+++ b/compat/tablesSchema.1.2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="660" windowWidth="13530" windowHeight="5475" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="438">
   <si>
     <t>Type</t>
   </si>
@@ -1182,9 +1182,6 @@
     <t>(RELATION{SummarizedInformation,type.code}!=RGT)</t>
   </si>
   <si>
-    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)</t>
-  </si>
-  <si>
     <t>IF_NOT_NULL(RELATION{CasesInformation,tseNationalCaseId.label},tseNationalCaseId=RELATION{CasesInformation,tseNationalCaseId.label}$,)|IF_NOT_NULL(RELATION{CasesInformation,tseIndexCase.code},tseIndexCase=RELATION{CasesInformation,tseIndexCase.code}$,)|IF_NOT_NULL(RELATION{CasesInformation,sampAnAsses.code},sampAnAsses=RELATION{CasesInformation,sampAnAsses.code},)|IF_NOT_NULL(RELATION{CasesInformation,evalCom.label},$com=RELATION{CasesInformation,evalCom.label},)</t>
   </si>
   <si>
@@ -1281,21 +1278,9 @@
     <t>IF((RELATION{SummarizedInformation,type.code}==RGT),SCRAPIE,)</t>
   </si>
   <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},)</t>
-  </si>
-  <si>
-    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}$RELATION{CasesInformation,animage.code}$RELATION{CasesInformation,sex.code}</t>
-  </si>
-  <si>
-    <t>psuId</t>
-  </si>
-  <si>
     <t>N123A</t>
   </si>
   <si>
-    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,psuId.label},$PSUId=RELATION{SummarizedInformation,psuId.label},)</t>
-  </si>
-  <si>
     <t>sexLists</t>
   </si>
   <si>
@@ -1308,9 +1293,6 @@
     <t>(RELATION{SummarizedInformation,type.code}!=CWD)</t>
   </si>
   <si>
-    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},)</t>
-  </si>
-  <si>
     <t>%progLegalRef.code|IF_NOT_NULL(RELATION{SummarizedInformation,tseTargetGroup.code},.|RELATION{SummarizedInformation,tseTargetGroup.code},)</t>
   </si>
   <si>
@@ -1335,7 +1317,28 @@
     <t>DO NOT TOUCH, used with Refresh Status/Display ack</t>
   </si>
   <si>
-    <t>HASH(MD5,%tseTargetGroup.code|%sampCountry.code|%sampY.code|%sampM.code|%source.code|%prod.code|%animage.code|%sex.code)</t>
+    <t>IF((RELATION{SummarizedInformation,type.code}!=RGT),RELATION{SummarizedInformation,animage.code},RELATION{CasesInformation,animage.code})</t>
+  </si>
+  <si>
+    <t>IF((RELATION{SummarizedInformation,type.code}==CWD),RELATION{SummarizedInformation,sex.code},RELATION{CasesInformation,sex.code})</t>
+  </si>
+  <si>
+    <t>A04MQ#RELATION{SummarizedInformation,source.code}$RELATION{CasesInformation,part.code}$RELATION{SummarizedInformation,prod.code}|IF_NOT_NULL(%animage.code,$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>A04MQ#%source.code$%prod.code|IF((%type.code!=RGT),$%animage.code,)|IF_NOT_NULL(%sex.code,$%sex.code,)</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(%PSUId.label,PSUId=%PSUId.label,)</t>
+  </si>
+  <si>
+    <t>PSUId</t>
+  </si>
+  <si>
+    <t>HASH(MD5,%tseTargetGroup.code|%sampCountry.code|%sampY.code|%sampM.code|%source.code|%prod.code|%animage.code|IF((%type.code==CWD),%sex.code,)|IF((%type.code==CWD),%PSUId.code,))</t>
+  </si>
+  <si>
+    <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
   </si>
 </sst>
 </file>
@@ -2962,8 +2965,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S33" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
-  <autoFilter ref="A1:S33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S34" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
+  <autoFilter ref="A1:S34"/>
   <sortState ref="A2:S32">
     <sortCondition ref="R1:R32"/>
   </sortState>
@@ -2995,8 +2998,8 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table2512" displayName="Table2512" ref="A1:S23" totalsRowShown="0" headerRowDxfId="60" dataDxfId="59">
   <autoFilter ref="A1:S23"/>
-  <sortState ref="A2:S22">
-    <sortCondition ref="R1:R22"/>
+  <sortState ref="A2:S23">
+    <sortCondition ref="R1:R23"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="58"/>
@@ -3024,10 +3027,10 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R37" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
-  <autoFilter ref="A1:R37"/>
-  <sortState ref="A2:R37">
-    <sortCondition ref="A1:A37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table25711" displayName="Table25711" ref="A1:R39" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+  <autoFilter ref="A1:R39"/>
+  <sortState ref="A2:R39">
+    <sortCondition ref="R1:R39"/>
   </sortState>
   <tableColumns count="18">
     <tableColumn id="1" name="id" dataDxfId="37"/>
@@ -4218,7 +4221,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4449,7 +4452,7 @@
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>176</v>
@@ -4480,13 +4483,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>176</v>
@@ -4517,13 +4520,13 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>176</v>
@@ -4562,7 +4565,7 @@
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4601,7 +4604,7 @@
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>176</v>
@@ -4632,15 +4635,15 @@
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>393</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>394</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>395</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24"/>
       <c r="E13" s="23" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>176</v>
@@ -4680,13 +4683,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,7 +4848,7 @@
         <v>319</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4994,43 +4997,43 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>414</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>415</v>
-      </c>
       <c r="I7" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>319</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="12" t="s">
@@ -5119,7 +5122,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -5157,7 +5160,7 @@
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -5195,7 +5198,7 @@
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -5233,7 +5236,7 @@
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -5247,7 +5250,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>176</v>
@@ -5271,12 +5274,12 @@
         <v>9</v>
       </c>
       <c r="R13" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
@@ -5326,7 +5329,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -5597,7 +5600,7 @@
         <v>4</v>
       </c>
       <c r="P23" s="12" t="s">
-        <v>385</v>
+        <v>433</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -5857,22 +5860,22 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="38" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>420</v>
+        <v>435</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J33" s="12" t="s">
         <v>3</v>
@@ -5881,7 +5884,33 @@
         <v>4</v>
       </c>
       <c r="R33" s="12">
-        <v>13</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J34" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P34" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="Q34" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -5898,10 +5927,10 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5986,163 +6015,166 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="B2" t="s">
-        <v>193</v>
+        <v>72</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>214</v>
+        <v>73</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>215</v>
+        <v>74</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>329</v>
+        <v>75</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>384</v>
+        <v>420</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>216</v>
+        <v>113</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>308</v>
+        <v>416</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>39</v>
+        <v>213</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="F3" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>8</v>
+        <v>215</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>329</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>3</v>
+        <v>384</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>66</v>
+        <v>201</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>68</v>
+        <v>202</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>389</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>390</v>
-      </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>3</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="B5" t="s">
-        <v>193</v>
+        <v>65</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>194</v>
+        <v>66</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>195</v>
+        <v>67</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>405</v>
+        <v>3</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>384</v>
+        <v>3</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>389</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S5" s="12" t="s">
         <v>9</v>
@@ -6150,51 +6182,57 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>203</v>
+        <v>411</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>204</v>
+        <v>58</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>205</v>
+        <v>412</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>206</v>
+        <v>412</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>12</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>8</v>
+        <v>413</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>432</v>
+        <v>4</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>3</v>
+        <v>421</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>3</v>
+        <v>421</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>419</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R6" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>204</v>
+        <v>192</v>
+      </c>
+      <c r="B7" t="s">
+        <v>193</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
@@ -6203,81 +6241,72 @@
         <v>8</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>4</v>
+        <v>404</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="23"/>
+        <v>384</v>
+      </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>36</v>
+        <v>203</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>35</v>
+        <v>204</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>372</v>
+        <v>205</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>4</v>
+        <v>426</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>431</v>
+        <v>3</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>431</v>
-      </c>
-      <c r="K8" s="27" t="s">
-        <v>109</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>408</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="K8" s="27"/>
       <c r="Q8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>7</v>
-      </c>
-      <c r="S8" s="12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>279</v>
+        <v>207</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>280</v>
+        <v>208</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>281</v>
+        <v>209</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
@@ -6299,148 +6328,149 @@
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>276</v>
+        <v>36</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>277</v>
+        <v>35</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>291</v>
+        <v>372</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>292</v>
+        <v>37</v>
       </c>
       <c r="F10" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="27"/>
+      <c r="G10" s="27" t="s">
+        <v>38</v>
+      </c>
       <c r="H10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>3</v>
+        <v>425</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>309</v>
+        <v>425</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>308</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>407</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R10" s="12">
+        <v>8</v>
+      </c>
+      <c r="S10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>217</v>
+        <v>279</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>219</v>
+        <v>280</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>220</v>
+        <v>281</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="23" t="s">
-        <v>221</v>
+        <v>176</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="I11" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="K11" s="12" t="s">
-        <v>222</v>
-      </c>
-      <c r="L11" s="12" t="s">
-        <v>223</v>
-      </c>
+      <c r="K11" s="23"/>
       <c r="Q11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="B12" t="s">
-        <v>193</v>
+        <v>276</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>277</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>197</v>
+        <v>291</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>198</v>
+        <v>292</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="23" t="s">
-        <v>199</v>
-      </c>
+      <c r="G12" s="23"/>
       <c r="H12" s="12" t="s">
-        <v>405</v>
+        <v>4</v>
       </c>
       <c r="I12" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>384</v>
+      <c r="J12" s="23" t="s">
+        <v>3</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>35</v>
+        <v>218</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>43</v>
+        <v>221</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>3</v>
@@ -6448,183 +6478,192 @@
       <c r="J13" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="O13"/>
-      <c r="P13"/>
+      <c r="K13" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>284</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>35</v>
+        <v>196</v>
+      </c>
+      <c r="B14" t="s">
+        <v>193</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>285</v>
+        <v>197</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="F14" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="11" t="s">
-        <v>287</v>
+      <c r="G14" s="23" t="s">
+        <v>199</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="I14" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="I14" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="11" t="s">
-        <v>392</v>
+      <c r="J14" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R14" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>288</v>
+        <v>210</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>289</v>
+        <v>211</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="F15" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="26"/>
+      <c r="G15" s="23" t="s">
+        <v>43</v>
+      </c>
       <c r="H15" s="12" t="s">
-        <v>432</v>
-      </c>
-      <c r="I15" s="26" t="s">
+        <v>426</v>
+      </c>
+      <c r="I15" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="K15" s="23" t="s">
-        <v>161</v>
-      </c>
+      <c r="K15" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="O15"/>
+      <c r="P15"/>
       <c r="Q15" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>377</v>
+        <v>285</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>314</v>
-      </c>
-      <c r="F16" s="23" t="s">
+        <v>286</v>
+      </c>
+      <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="12" t="s">
-        <v>199</v>
+      <c r="G16" s="11" t="s">
+        <v>287</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I16" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="J16" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="26" t="s">
-        <v>283</v>
+      <c r="K16" s="11" t="s">
+        <v>391</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R16" s="12">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>274</v>
+        <v>35</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>295</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>8</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="26"/>
       <c r="H17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="I17" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="J17" s="26" t="s">
         <v>3</v>
       </c>
+      <c r="K17" s="23" t="s">
+        <v>161</v>
+      </c>
       <c r="Q17" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R17" s="12">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>193</v>
+        <v>35</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>297</v>
+        <v>377</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>298</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>176</v>
+        <v>314</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>12</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>4</v>
@@ -6635,80 +6674,89 @@
       <c r="J18" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K18" s="26" t="s">
+        <v>283</v>
+      </c>
       <c r="Q18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R18" s="12">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>412</v>
+        <v>293</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>58</v>
+        <v>274</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>413</v>
+        <v>294</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>413</v>
+        <v>295</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>414</v>
+        <v>8</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>426</v>
+        <v>3</v>
       </c>
       <c r="J19" s="12" t="s">
-        <v>426</v>
-      </c>
-      <c r="K19" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="L19" s="12" t="s">
-        <v>424</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>427</v>
+        <v>3</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R19" s="12">
-        <v>-1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>224</v>
+        <v>296</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>298</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I20" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="R20" s="12">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>175</v>
@@ -6728,13 +6776,10 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>355</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>356</v>
+        <v>174</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>4</v>
@@ -6743,9 +6788,6 @@
         <v>4</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O22" s="12" t="s">
         <v>4</v>
       </c>
       <c r="Q22" s="12" t="s">
@@ -6754,46 +6796,28 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>73</v>
+        <v>355</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>74</v>
+        <v>356</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>75</v>
+        <v>176</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>425</v>
+        <v>4</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>425</v>
+        <v>4</v>
       </c>
       <c r="J23" s="12" t="s">
-        <v>425</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>417</v>
-      </c>
-      <c r="M23" s="12" t="s">
-        <v>418</v>
+        <v>4</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>5</v>
-      </c>
-      <c r="R23" s="12">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6807,13 +6831,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6895,101 +6919,110 @@
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>270</v>
+        <v>97</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>84</v>
+        <v>96</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>269</v>
+        <v>397</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>406</v>
+        <v>3</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>409</v>
+        <v>3</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>409</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>410</v>
+        <v>3</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>374</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R2" s="12">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>267</v>
+        <v>91</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>91</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>92</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>406</v>
+        <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>409</v>
+        <v>3</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>409</v>
+        <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="L3" s="13" t="s">
-        <v>410</v>
+        <v>313</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>308</v>
       </c>
       <c r="Q3" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="R3" s="12">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>271</v>
+        <v>144</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>380</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>242</v>
+        <v>12</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
@@ -7001,180 +7034,198 @@
         <v>3</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>391</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>299</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>302</v>
+        <v>114</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>370</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="R4" s="12">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>94</v>
+        <v>349</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>380</v>
+        <v>257</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>3</v>
+        <v>351</v>
       </c>
       <c r="I5" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>3</v>
+        <v>384</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>114</v>
+        <v>348</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>370</v>
+        <v>350</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>176</v>
+        <v>242</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>318</v>
+        <v>3</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="M6" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>9</v>
+      </c>
+      <c r="R6" s="12">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>91</v>
+        <v>270</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>3</v>
+        <v>405</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>3</v>
+        <v>408</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>3</v>
+        <v>408</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>313</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>308</v>
+        <v>328</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>409</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>230</v>
+        <v>267</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>265</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>175</v>
+        <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>4</v>
+        <v>405</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>4</v>
+        <v>408</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>4</v>
+        <v>408</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>409</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
+      </c>
+      <c r="R8" s="12">
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>229</v>
+        <v>89</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>229</v>
+        <v>89</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G9" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H9" s="12" t="s">
         <v>4</v>
       </c>
@@ -7184,8 +7235,8 @@
       <c r="J9" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>386</v>
+      <c r="N9" s="12" t="s">
+        <v>318</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -7193,22 +7244,10 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>332</v>
+        <v>230</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>8</v>
+        <v>175</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>4</v>
@@ -7219,19 +7258,22 @@
       <c r="J10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P10" s="12" t="s">
-        <v>331</v>
-      </c>
       <c r="Q10" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>332</v>
+        <v>229</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>176</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>4</v>
@@ -7242,28 +7284,31 @@
       <c r="J11" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M11" s="12" t="s">
-        <v>402</v>
+      <c r="P11" s="12" t="s">
+        <v>385</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>81</v>
+        <v>85</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>332</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>4</v>
@@ -7274,11 +7319,8 @@
       <c r="J12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="O12" s="12" t="s">
-        <v>228</v>
+      <c r="P12" s="12" t="s">
+        <v>331</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -7286,19 +7328,10 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>8</v>
+        <v>330</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>332</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>4</v>
@@ -7309,22 +7342,28 @@
       <c r="J13" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P13" s="12" t="s">
-        <v>429</v>
+      <c r="M13" s="12" t="s">
+        <v>401</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>403</v>
+        <v>81</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>4</v>
@@ -7335,22 +7374,25 @@
       <c r="J14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P14" s="12" t="s">
-        <v>428</v>
+      <c r="M14" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
@@ -7368,7 +7410,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>387</v>
+        <v>423</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7376,25 +7418,13 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>397</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>4</v>
@@ -7405,179 +7435,179 @@
       <c r="J16" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="12" t="s">
-        <v>421</v>
+      <c r="P16" s="12" t="s">
+        <v>422</v>
       </c>
       <c r="Q16" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G17" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P17" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q17" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>398</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M18" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="Q18" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N17" s="12" t="s">
+      <c r="H19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N19" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="Q17" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="Q19" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F20" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="H18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J18" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+      <c r="H20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C21" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F21" s="12" t="s">
         <v>242</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G21" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J19" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N19" s="12" t="s">
+      <c r="H21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N21" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="Q19" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="O20" s="12" t="s">
-        <v>374</v>
-      </c>
-      <c r="Q20" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="R20" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
+      <c r="Q21" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B22" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C22" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E22" s="28" t="s">
         <v>332</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M21" s="12" t="s">
-        <v>404</v>
-      </c>
-      <c r="Q21" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>255</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>255</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
@@ -7592,28 +7622,25 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>254</v>
+        <v>403</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>77</v>
+        <v>255</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>76</v>
+        <v>256</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>77</v>
+        <v>255</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G23" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="H23" s="12" t="s">
         <v>4</v>
       </c>
@@ -7623,28 +7650,28 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P23" s="12" t="s">
-        <v>272</v>
+      <c r="M23" s="12" t="s">
+        <v>254</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>217</v>
+        <v>77</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>218</v>
+        <v>76</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>217</v>
+        <v>77</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>221</v>
+        <v>8</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>4</v>
@@ -7655,89 +7682,89 @@
       <c r="J24" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N24" s="12" t="s">
-        <v>278</v>
+      <c r="P24" s="12" t="s">
+        <v>272</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>45</v>
+        <v>217</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>44</v>
+        <v>218</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>45</v>
+        <v>217</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q25" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G26" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="H25" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I25" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N25" s="12" t="s">
+      <c r="H26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N26" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="Q25" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="Q26" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B27" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C27" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>242</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>275</v>
-      </c>
-      <c r="Q26" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>176</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>8</v>
@@ -7751,26 +7778,29 @@
       <c r="J27" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P27" s="12" t="s">
-        <v>383</v>
+      <c r="N27" s="12" t="s">
+        <v>275</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>99</v>
+        <v>34</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G28" s="12" t="s">
+        <v>8</v>
+      </c>
       <c r="H28" s="12" t="s">
         <v>4</v>
       </c>
@@ -7781,34 +7811,25 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>371</v>
+        <v>383</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>202</v>
+        <v>99</v>
       </c>
       <c r="F29" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>8</v>
-      </c>
       <c r="H29" s="12" t="s">
         <v>4</v>
       </c>
@@ -7819,24 +7840,30 @@
         <v>4</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>272</v>
+        <v>371</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>52</v>
+        <v>40</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>202</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G30" s="12" t="s">
         <v>8</v>
@@ -7850,58 +7877,61 @@
       <c r="J30" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N30" s="12" t="s">
+      <c r="P30" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N31" s="12" t="s">
         <v>300</v>
       </c>
-      <c r="Q30" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="Q31" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="12" t="s">
+      <c r="B32" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="G31" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P31" s="12" t="s">
-        <v>419</v>
-      </c>
-      <c r="Q31" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12" t="s">
-        <v>273</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>273</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>176</v>
       </c>
+      <c r="G32" s="12" t="s">
+        <v>60</v>
+      </c>
       <c r="H32" s="12" t="s">
         <v>4</v>
       </c>
@@ -7912,28 +7942,25 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>307</v>
+        <v>432</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>55</v>
+        <v>273</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>54</v>
+        <v>274</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>55</v>
+        <v>273</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G33" s="12" t="s">
-        <v>56</v>
-      </c>
       <c r="H33" s="12" t="s">
         <v>4</v>
       </c>
@@ -7943,31 +7970,28 @@
       <c r="J33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M33" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O33" s="12" t="s">
-        <v>57</v>
+      <c r="P33" s="12" t="s">
+        <v>307</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>204</v>
+        <v>54</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G34" s="12" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>4</v>
@@ -7978,25 +8002,28 @@
       <c r="J34" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P34" s="12" t="s">
-        <v>422</v>
+      <c r="M34" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O34" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>49</v>
+        <v>226</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>48</v>
+        <v>204</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>49</v>
+        <v>226</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>8</v>
@@ -8010,66 +8037,115 @@
       <c r="J35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N35" s="12" t="s">
+      <c r="P35" s="12" t="s">
+        <v>437</v>
+      </c>
+      <c r="Q35" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N36" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="Q35" s="12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="Q36" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12" t="s">
         <v>224</v>
       </c>
-      <c r="F36" s="12" t="s">
+      <c r="F37" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="H36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J36" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q36" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="12" t="s">
-        <v>349</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="F37" s="12" t="s">
+      <c r="H37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q37" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="G37" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>351</v>
-      </c>
-      <c r="I37" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>348</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>350</v>
-      </c>
-      <c r="Q37" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="R37" s="12">
-        <v>4</v>
+      <c r="H38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J38" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N38" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q38" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J39" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="N39" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="Q39" s="12" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -8668,7 +8744,7 @@
         <v>376</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8724,7 +8800,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>353</v>

</xml_diff>

<commit_message>
changed editability of some fixed fields for RGT. Fixed age class validator for RGT. Fixed some bugs
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.0.xlsx
+++ b/compat/tablesSchema.1.2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -4685,11 +4685,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4836,7 +4836,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>3</v>
+        <v>382</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>3</v>
@@ -4883,7 +4883,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>3</v>
+        <v>382</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>3</v>
@@ -6833,11 +6833,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7063,7 +7063,7 @@
         <v>351</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>3</v>
+        <v>351</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>384</v>
@@ -7148,7 +7148,7 @@
         <v>405</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>408</v>
@@ -7186,7 +7186,7 @@
         <v>405</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>408</v>

</xml_diff>

<commit_message>
fixed bug of report importer. breed and evalCol were ignored during the import
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.0.xlsx
+++ b/compat/tablesSchema.1.2.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="720" windowWidth="13530" windowHeight="5415" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="439">
   <si>
     <t>Type</t>
   </si>
@@ -1339,6 +1339,9 @@
   </si>
   <si>
     <t>IF_NOT_NULL(RELATION{CasesInformation,animalId.code},animalId=RELATION{CasesInformation,animalId.code},)|IF_NOT_NULL(RELATION{CasesInformation,herdId.label},$herdId=RELATION{CasesInformation,herdId.label}, )|IF_NOT_NULL(RELATION{CasesInformation,sampHoldingId.label},$sampHoldingId=RELATION{CasesInformation,sampHoldingId.label},)|IF_NOT_NULL(RELATION{SummarizedInformation,PSUId.label},$PSUId=RELATION{SummarizedInformation,PSUId.label},)</t>
+  </si>
+  <si>
+    <t>AND((RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
   </si>
 </sst>
 </file>
@@ -4685,7 +4688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -5926,11 +5929,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S5" sqref="S5"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6357,7 +6360,7 @@
         <v>425</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>425</v>
+        <v>438</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>109</v>
@@ -6834,10 +6837,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added analysis year check and changed part picklist
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.0.xlsx
+++ b/compat/tablesSchema.1.2.0.xlsx
@@ -669,9 +669,6 @@
     <t>sampAnAsses</t>
   </si>
   <si>
-    <t>Case assessment</t>
-  </si>
-  <si>
     <t>Final evaluation of the case after discriminatory testing</t>
   </si>
   <si>
@@ -1342,6 +1339,9 @@
   </si>
   <si>
     <t>AND((RELATION{SummarizedInformation,prod.code}==F21.A07RV),(RELATION{SummarizedInformation,type.code}!=RGT))</t>
+  </si>
+  <si>
+    <t>Sample/case assessment</t>
   </si>
 </sst>
 </file>
@@ -2970,8 +2970,8 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:S34" totalsRowShown="0" headerRowDxfId="81" dataDxfId="80">
   <autoFilter ref="A1:S34"/>
-  <sortState ref="A2:S32">
-    <sortCondition ref="R1:R32"/>
+  <sortState ref="A2:S34">
+    <sortCondition ref="R1:R34"/>
   </sortState>
   <tableColumns count="19">
     <tableColumn id="1" name="id" dataDxfId="79"/>
@@ -3750,7 +3750,7 @@
         <v>123</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>12</v>
@@ -3771,7 +3771,7 @@
         <v>114</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="R3">
         <v>2</v>
@@ -3789,7 +3789,7 @@
         <v>125</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>12</v>
@@ -3810,7 +3810,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="R4">
         <v>3</v>
@@ -3828,7 +3828,7 @@
         <v>127</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>12</v>
@@ -3849,7 +3849,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="R5">
         <v>4</v>
@@ -3888,7 +3888,7 @@
         <v>114</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="R6">
         <v>5</v>
@@ -3927,7 +3927,7 @@
         <v>114</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="R7">
         <v>6</v>
@@ -3966,7 +3966,7 @@
         <v>114</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R8">
         <v>7</v>
@@ -3974,17 +3974,17 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>12</v>
@@ -4005,7 +4005,7 @@
         <v>114</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="R9">
         <v>8</v>
@@ -4013,17 +4013,17 @@
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>12</v>
@@ -4044,7 +4044,7 @@
         <v>114</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="R10">
         <v>9</v>
@@ -4052,17 +4052,17 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F11" s="33" t="s">
         <v>12</v>
@@ -4083,7 +4083,7 @@
         <v>114</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M11" s="32"/>
       <c r="N11" s="32"/>
@@ -4212,7 +4212,7 @@
         <v>12</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>9</v>
@@ -4224,7 +4224,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="14" t="s">
@@ -4305,7 +4305,7 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
@@ -4326,10 +4326,10 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
       <c r="O4" s="12" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P4" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>5</v>
@@ -4375,11 +4375,11 @@
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P5" s="16"/>
       <c r="Q5" s="16" t="s">
@@ -4417,13 +4417,13 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
+        <v>324</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>325</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>243</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>326</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>176</v>
@@ -4447,15 +4447,15 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>176</v>
@@ -4486,13 +4486,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>176</v>
@@ -4523,13 +4523,13 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>176</v>
@@ -4560,15 +4560,15 @@
     </row>
     <row r="11" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="23" t="s">
         <v>250</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>251</v>
       </c>
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4599,15 +4599,15 @@
     </row>
     <row r="12" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B12" s="23" t="s">
         <v>245</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>246</v>
       </c>
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>176</v>
@@ -4638,15 +4638,15 @@
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>392</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>393</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>394</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24"/>
       <c r="E13" s="23" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>176</v>
@@ -4692,7 +4692,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4807,7 +4807,7 @@
         <v>146</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
@@ -4839,7 +4839,7 @@
         <v>3</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J3" s="12" t="s">
         <v>3</v>
@@ -4848,10 +4848,10 @@
         <v>110</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -4871,7 +4871,7 @@
         <v>58</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>70</v>
@@ -4886,7 +4886,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J4" s="12" t="s">
         <v>3</v>
@@ -4895,10 +4895,10 @@
         <v>112</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M4" s="12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
@@ -4930,10 +4930,10 @@
         <v>75</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J5" s="12" t="s">
         <v>3</v>
@@ -4942,7 +4942,7 @@
         <v>113</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -4974,10 +4974,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J6" s="12" t="s">
         <v>3</v>
@@ -4986,7 +4986,7 @@
         <v>108</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -5000,43 +5000,43 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>414</v>
-      </c>
       <c r="I7" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L7" s="12" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="12" t="s">
@@ -5050,238 +5050,238 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>25</v>
+      <c r="A8" s="38" t="s">
+        <v>434</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>14</v>
+        <v>204</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>378</v>
+        <v>434</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>8</v>
+        <v>176</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>382</v>
+        <v>413</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>382</v>
+        <v>413</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O8" s="12" t="s">
-        <v>381</v>
-      </c>
       <c r="Q8" s="12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R8" s="12">
         <v>7</v>
       </c>
-      <c r="S8" s="12" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>24</v>
+        <v>377</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J9" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R9" s="12">
+        <v>8</v>
+      </c>
+      <c r="S9" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>379</v>
+        <v>29</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>4</v>
+        <v>381</v>
       </c>
       <c r="J11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="12" t="s">
-        <v>316</v>
+      <c r="O11" s="12" t="s">
+        <v>380</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>32</v>
+        <v>378</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G12" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>382</v>
+        <v>4</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>382</v>
+        <v>4</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="O12" s="12" t="s">
-        <v>381</v>
+      <c r="P12" s="12" t="s">
+        <v>315</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>400</v>
+        <v>31</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>32</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>3</v>
+        <v>381</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>4</v>
+        <v>381</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>3</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>327</v>
+        <v>380</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>399</v>
       </c>
       <c r="F14" s="12" t="s">
@@ -5291,30 +5291,27 @@
         <v>8</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>436</v>
+        <v>3</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>326</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="R14" s="12">
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>15</v>
+        <v>398</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
@@ -5332,21 +5329,21 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>387</v>
+        <v>435</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -5364,7 +5361,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>317</v>
+        <v>386</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>9</v>
@@ -5372,19 +5369,19 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F17" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>4</v>
@@ -5395,11 +5392,8 @@
       <c r="J17" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N17" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="P17" s="12" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -5407,13 +5401,13 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -5431,10 +5425,10 @@
         <v>4</v>
       </c>
       <c r="N18" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -5442,19 +5436,19 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>4</v>
@@ -5466,10 +5460,10 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>299</v>
+        <v>222</v>
       </c>
       <c r="P19" s="12" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -5477,16 +5471,16 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>8</v>
@@ -5500,8 +5494,11 @@
       <c r="J20" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="N20" s="12" t="s">
+        <v>298</v>
+      </c>
       <c r="P20" s="12" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="Q20" s="12" t="s">
         <v>9</v>
@@ -5509,16 +5506,16 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>8</v>
@@ -5532,11 +5529,8 @@
       <c r="J21" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="N21" s="12" t="s">
-        <v>300</v>
-      </c>
       <c r="P21" s="12" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -5544,19 +5538,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>4</v>
@@ -5567,11 +5561,11 @@
       <c r="J22" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M22" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="O22" s="12" t="s">
-        <v>57</v>
+      <c r="N22" s="12" t="s">
+        <v>299</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>302</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -5579,19 +5573,19 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>4</v>
@@ -5602,8 +5596,11 @@
       <c r="J23" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P23" s="12" t="s">
-        <v>433</v>
+      <c r="M23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="O23" s="12" t="s">
+        <v>57</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -5611,19 +5608,19 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="H24" s="12" t="s">
         <v>4</v>
@@ -5635,7 +5632,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>317</v>
+        <v>432</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -5643,16 +5640,16 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>8</v>
@@ -5667,7 +5664,7 @@
         <v>4</v>
       </c>
       <c r="P25" s="12" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -5675,19 +5672,19 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>176</v>
+        <v>241</v>
       </c>
       <c r="G26" s="12" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>4</v>
@@ -5698,11 +5695,8 @@
       <c r="J26" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="O26" s="12" t="s">
-        <v>83</v>
+      <c r="P26" s="12" t="s">
+        <v>314</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
@@ -5710,19 +5704,19 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H27" s="12" t="s">
         <v>4</v>
@@ -5734,10 +5728,10 @@
         <v>4</v>
       </c>
       <c r="M27" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="O27" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
@@ -5745,19 +5739,19 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F28" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="H28" s="12" t="s">
         <v>4</v>
@@ -5768,8 +5762,11 @@
       <c r="J28" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="P28" s="12" t="s">
-        <v>320</v>
+      <c r="M28" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="O28" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -5777,10 +5774,19 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>174</v>
+        <v>97</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>97</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>8</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>4</v>
@@ -5791,13 +5797,16 @@
       <c r="J29" s="12" t="s">
         <v>4</v>
       </c>
+      <c r="P29" s="12" t="s">
+        <v>319</v>
+      </c>
       <c r="Q29" s="12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>175</v>
@@ -5817,7 +5826,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>175</v>
@@ -5837,65 +5846,56 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q32" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="E33" s="12" t="s">
         <v>355</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>356</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="O32" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q32" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
-        <v>435</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>435</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>414</v>
+        <v>4</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>414</v>
+        <v>4</v>
       </c>
       <c r="J33" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O33" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="R33" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>176</v>
@@ -5910,7 +5910,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>9</v>
@@ -5930,10 +5930,10 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="A5:R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6018,210 +6018,210 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>58</v>
+        <v>213</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>73</v>
+        <v>438</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>74</v>
+        <v>214</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>75</v>
+        <v>328</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>113</v>
+        <v>215</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>416</v>
+        <v>307</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R2" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" t="s">
-        <v>193</v>
+        <v>40</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>39</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>215</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>329</v>
+        <v>202</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>8</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="J3" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="K3" s="12" t="s">
-        <v>216</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>308</v>
+        <v>3</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>3</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R3" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>201</v>
+        <v>66</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="F4" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>8</v>
+        <v>67</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>68</v>
       </c>
       <c r="H4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="I4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="12" t="s">
         <v>3</v>
       </c>
+      <c r="K4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>387</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>388</v>
+      </c>
       <c r="Q4" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="12">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>65</v>
+        <v>410</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>66</v>
+        <v>411</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>67</v>
+        <v>411</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>68</v>
+        <v>412</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>3</v>
+        <v>420</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>3</v>
+        <v>420</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>111</v>
+        <v>417</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>308</v>
-      </c>
-      <c r="M5" s="12" t="s">
-        <v>388</v>
-      </c>
-      <c r="O5" s="12" t="s">
-        <v>389</v>
+        <v>418</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R5" s="12">
-        <v>3</v>
-      </c>
-      <c r="S5" s="12" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>411</v>
+        <v>72</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>412</v>
+        <v>73</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>412</v>
+        <v>74</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>413</v>
+        <v>75</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>4</v>
+        <v>419</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>418</v>
+        <v>113</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R6" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -6244,19 +6244,19 @@
         <v>8</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R7" s="12">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S7" s="12" t="s">
         <v>9</v>
@@ -6282,7 +6282,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>3</v>
@@ -6295,7 +6295,7 @@
         <v>5</v>
       </c>
       <c r="R8" s="12">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -6331,7 +6331,7 @@
         <v>5</v>
       </c>
       <c r="R9" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -6342,7 +6342,7 @@
         <v>35</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>37</v>
@@ -6357,25 +6357,25 @@
         <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>109</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R10" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="S10" s="12" t="s">
         <v>9</v>
@@ -6383,16 +6383,16 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D11" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="E11" s="12" t="s">
         <v>280</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>281</v>
       </c>
       <c r="F11" s="27" t="s">
         <v>176</v>
@@ -6414,21 +6414,21 @@
         <v>5</v>
       </c>
       <c r="R11" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B12" s="12" t="s">
-        <v>277</v>
-      </c>
       <c r="D12" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>291</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>292</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>12</v>
@@ -6444,36 +6444,36 @@
         <v>3</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R12" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="D13" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="E13" s="12" t="s">
         <v>219</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>220</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>3</v>
@@ -6482,16 +6482,16 @@
         <v>3</v>
       </c>
       <c r="K13" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="L13" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="L13" s="12" t="s">
-        <v>223</v>
-      </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R13" s="12">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -6514,25 +6514,25 @@
         <v>199</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>3</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K14" s="12" t="s">
         <v>200</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R14" s="12">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -6555,7 +6555,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>3</v>
@@ -6572,30 +6572,30 @@
         <v>5</v>
       </c>
       <c r="R15" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D16" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="E16" s="12" t="s">
         <v>285</v>
-      </c>
-      <c r="E16" s="12" t="s">
-        <v>286</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>3</v>
@@ -6604,34 +6604,34 @@
         <v>3</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R16" s="12">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>289</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>290</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>12</v>
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="12" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I17" s="26" t="s">
         <v>3</v>
@@ -6646,21 +6646,21 @@
         <v>5</v>
       </c>
       <c r="R17" s="12">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F18" s="23" t="s">
         <v>12</v>
@@ -6678,27 +6678,27 @@
         <v>3</v>
       </c>
       <c r="K18" s="26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>5</v>
       </c>
       <c r="R18" s="12">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>293</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>274</v>
-      </c>
-      <c r="D19" s="12" t="s">
+      <c r="E19" s="12" t="s">
         <v>294</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>295</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>176</v>
@@ -6719,21 +6719,21 @@
         <v>5</v>
       </c>
       <c r="R19" s="12">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>193</v>
       </c>
       <c r="D20" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="E20" s="12" t="s">
         <v>297</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>298</v>
       </c>
       <c r="F20" s="12" t="s">
         <v>176</v>
@@ -6754,12 +6754,12 @@
         <v>5</v>
       </c>
       <c r="R20" s="12">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F21" s="12" t="s">
         <v>175</v>
@@ -6799,10 +6799,10 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>354</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>355</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>356</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
@@ -6837,10 +6837,10 @@
   <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P33" sqref="P33"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6931,10 +6931,10 @@
         <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>176</v>
@@ -6952,7 +6952,7 @@
         <v>3</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>9</v>
@@ -6972,10 +6972,10 @@
         <v>91</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>176</v>
@@ -6993,10 +6993,10 @@
         <v>3</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="L3" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>9</v>
@@ -7019,7 +7019,7 @@
         <v>144</v>
       </c>
       <c r="E4" s="36" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>12</v>
@@ -7040,7 +7040,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="Q4" s="12" t="s">
         <v>9</v>
@@ -7051,10 +7051,10 @@
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>176</v>
@@ -7063,19 +7063,19 @@
         <v>86</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -7095,13 +7095,13 @@
         <v>79</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>8</v>
@@ -7116,13 +7116,13 @@
         <v>3</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="O6" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>9</v>
@@ -7133,34 +7133,34 @@
     </row>
     <row r="7" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J7" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>408</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>409</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -7171,34 +7171,34 @@
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>84</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="J8" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="L8" s="13" t="s">
         <v>408</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>328</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>409</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -7218,10 +7218,10 @@
         <v>89</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F9" s="12" t="s">
         <v>176</v>
@@ -7239,7 +7239,7 @@
         <v>4</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="Q9" s="12" t="s">
         <v>9</v>
@@ -7247,7 +7247,7 @@
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>175</v>
@@ -7267,13 +7267,13 @@
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>193</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>176</v>
@@ -7288,7 +7288,7 @@
         <v>4</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q11" s="12" t="s">
         <v>9</v>
@@ -7305,7 +7305,7 @@
         <v>85</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F12" s="12" t="s">
         <v>176</v>
@@ -7323,7 +7323,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q12" s="12" t="s">
         <v>9</v>
@@ -7331,10 +7331,10 @@
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H13" s="12" t="s">
         <v>4</v>
@@ -7346,7 +7346,7 @@
         <v>4</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -7378,10 +7378,10 @@
         <v>4</v>
       </c>
       <c r="M14" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O14" s="12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q14" s="12" t="s">
         <v>9</v>
@@ -7413,7 +7413,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7421,7 +7421,7 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -7439,7 +7439,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -7471,7 +7471,7 @@
         <v>4</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="Q17" s="12" t="s">
         <v>9</v>
@@ -7488,10 +7488,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -7509,7 +7509,7 @@
         <v>4</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -7541,7 +7541,7 @@
         <v>4</v>
       </c>
       <c r="N19" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q19" s="12" t="s">
         <v>9</v>
@@ -7578,7 +7578,7 @@
         <v>47</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G21" s="12" t="s">
         <v>8</v>
@@ -7593,7 +7593,7 @@
         <v>4</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q21" s="12" t="s">
         <v>9</v>
@@ -7601,16 +7601,16 @@
     </row>
     <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="B22" s="12" t="s">
-        <v>259</v>
-      </c>
       <c r="C22" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E22" s="28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F22" s="12" t="s">
         <v>176</v>
@@ -7625,7 +7625,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -7633,13 +7633,13 @@
     </row>
     <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B23" s="12" t="s">
         <v>255</v>
       </c>
-      <c r="B23" s="12" t="s">
-        <v>256</v>
-      </c>
       <c r="C23" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F23" s="12" t="s">
         <v>176</v>
@@ -7654,7 +7654,7 @@
         <v>4</v>
       </c>
       <c r="M23" s="12" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q23" s="12" t="s">
         <v>9</v>
@@ -7686,7 +7686,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -7694,19 +7694,19 @@
     </row>
     <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>218</v>
-      </c>
       <c r="C25" s="12" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>176</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>4</v>
@@ -7718,7 +7718,7 @@
         <v>4</v>
       </c>
       <c r="N25" s="12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="Q25" s="12" t="s">
         <v>9</v>
@@ -7750,7 +7750,7 @@
         <v>4</v>
       </c>
       <c r="N26" s="12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="Q26" s="12" t="s">
         <v>9</v>
@@ -7758,16 +7758,16 @@
     </row>
     <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B27" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B27" s="12" t="s">
-        <v>277</v>
-      </c>
       <c r="C27" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G27" s="12" t="s">
         <v>8</v>
@@ -7782,7 +7782,7 @@
         <v>4</v>
       </c>
       <c r="N27" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="Q27" s="12" t="s">
         <v>9</v>
@@ -7814,7 +7814,7 @@
         <v>4</v>
       </c>
       <c r="P28" s="12" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="Q28" s="12" t="s">
         <v>9</v>
@@ -7843,7 +7843,7 @@
         <v>4</v>
       </c>
       <c r="P29" s="12" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q29" s="12" t="s">
         <v>9</v>
@@ -7881,7 +7881,7 @@
         <v>4</v>
       </c>
       <c r="P30" s="12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="Q30" s="12" t="s">
         <v>9</v>
@@ -7898,7 +7898,7 @@
         <v>52</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G31" s="12" t="s">
         <v>8</v>
@@ -7913,7 +7913,7 @@
         <v>4</v>
       </c>
       <c r="N31" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="Q31" s="12" t="s">
         <v>9</v>
@@ -7945,7 +7945,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
@@ -7953,13 +7953,13 @@
     </row>
     <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="B33" s="12" t="s">
         <v>273</v>
       </c>
-      <c r="B33" s="12" t="s">
-        <v>274</v>
-      </c>
       <c r="C33" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F33" s="12" t="s">
         <v>176</v>
@@ -7974,7 +7974,7 @@
         <v>4</v>
       </c>
       <c r="P33" s="12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q33" s="12" t="s">
         <v>9</v>
@@ -8017,13 +8017,13 @@
     </row>
     <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>204</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F35" s="12" t="s">
         <v>176</v>
@@ -8041,7 +8041,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>9</v>
@@ -8058,7 +8058,7 @@
         <v>49</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G36" s="12" t="s">
         <v>8</v>
@@ -8073,7 +8073,7 @@
         <v>4</v>
       </c>
       <c r="N36" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="Q36" s="12" t="s">
         <v>9</v>
@@ -8081,7 +8081,7 @@
     </row>
     <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="F37" s="12" t="s">
         <v>175</v>
@@ -8101,7 +8101,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>58</v>
@@ -8119,7 +8119,7 @@
         <v>4</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q38" s="12" t="s">
         <v>5</v>
@@ -8145,7 +8145,7 @@
         <v>4</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q39" s="12" t="s">
         <v>5</v>
@@ -8182,7 +8182,7 @@
         <v>171</v>
       </c>
       <c r="C1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -8190,7 +8190,7 @@
         <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -8201,7 +8201,7 @@
         <v>173</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
@@ -8253,10 +8253,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -8267,7 +8267,7 @@
         <v>172</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -8278,7 +8278,7 @@
         <v>173</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -8289,7 +8289,7 @@
         <v>172</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -8300,7 +8300,7 @@
         <v>177</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -8340,7 +8340,7 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -8369,18 +8369,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -8510,7 +8510,7 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P2" s="11"/>
       <c r="Q2" s="2" t="s">
@@ -8521,11 +8521,11 @@
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -8545,7 +8545,7 @@
       <c r="M3" s="14"/>
       <c r="N3" s="14"/>
       <c r="O3" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P3" s="11"/>
       <c r="Q3" s="2" t="s">
@@ -8556,11 +8556,11 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -8579,7 +8579,7 @@
       <c r="L4" s="2"/>
       <c r="M4" s="12"/>
       <c r="P4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>3</v>
@@ -8589,11 +8589,11 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -8612,7 +8612,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="16"/>
       <c r="P5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>3</v>
@@ -8622,10 +8622,10 @@
     </row>
     <row r="6" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>176</v>
@@ -8637,7 +8637,7 @@
         <v>4</v>
       </c>
       <c r="O6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>3</v>
@@ -8645,10 +8645,10 @@
     </row>
     <row r="7" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F7" s="7" t="s">
         <v>176</v>
@@ -8661,7 +8661,7 @@
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="12" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>3</v>
@@ -8669,10 +8669,10 @@
     </row>
     <row r="8" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>176</v>
@@ -8685,7 +8685,7 @@
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="12" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>3</v>
@@ -8693,10 +8693,10 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F9" s="7" t="s">
         <v>176</v>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>3</v>
@@ -8717,15 +8717,15 @@
     </row>
     <row r="10" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="16"/>
       <c r="C10" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D10" s="16"/>
       <c r="E10" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>176</v>
@@ -8744,10 +8744,10 @@
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
       <c r="P10" s="37" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8777,7 +8777,7 @@
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="P11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>3</v>
@@ -8787,10 +8787,10 @@
     </row>
     <row r="12" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="2" t="s">
@@ -8803,18 +8803,18 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>176</v>
@@ -8832,13 +8832,13 @@
     </row>
     <row r="14" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>322</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="E14" s="35" t="s">
-        <v>323</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
changed lymph code and some default values
</commit_message>
<xml_diff>
--- a/compat/tablesSchema.1.2.0.xlsx
+++ b/compat/tablesSchema.1.2.0.xlsx
@@ -1200,9 +1200,6 @@
     <t>animalYearsList</t>
   </si>
   <si>
-    <t>IF((%type.code==RGT),F01.A057G,)</t>
-  </si>
-  <si>
     <t>reportPreviousStatus</t>
   </si>
   <si>
@@ -1342,6 +1339,9 @@
   </si>
   <si>
     <t>Sample/case assessment</t>
+  </si>
+  <si>
+    <t>IF((%type.code==RGT),F01.A057G,)IF((%type.code==BSE),F01.A057E,)</t>
   </si>
 </sst>
 </file>
@@ -4455,7 +4455,7 @@
       <c r="C8" s="23"/>
       <c r="D8" s="24"/>
       <c r="E8" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F8" s="23" t="s">
         <v>176</v>
@@ -4486,13 +4486,13 @@
     </row>
     <row r="9" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
       <c r="D9" s="24"/>
       <c r="E9" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F9" s="23" t="s">
         <v>176</v>
@@ -4523,13 +4523,13 @@
     </row>
     <row r="10" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
       <c r="D10" s="24"/>
       <c r="E10" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F10" s="23" t="s">
         <v>176</v>
@@ -4568,7 +4568,7 @@
       <c r="C11" s="23"/>
       <c r="D11" s="24"/>
       <c r="E11" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F11" s="23" t="s">
         <v>176</v>
@@ -4607,7 +4607,7 @@
       <c r="C12" s="23"/>
       <c r="D12" s="24"/>
       <c r="E12" s="23" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>176</v>
@@ -4638,15 +4638,15 @@
     </row>
     <row r="13" spans="1:19" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
+        <v>391</v>
+      </c>
+      <c r="B13" s="23" t="s">
         <v>392</v>
-      </c>
-      <c r="B13" s="23" t="s">
-        <v>393</v>
       </c>
       <c r="C13" s="23"/>
       <c r="D13" s="24"/>
       <c r="E13" s="23" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F13" s="23" t="s">
         <v>176</v>
@@ -4692,7 +4692,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R35" sqref="R35"/>
+      <selection pane="bottomRight" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4851,7 +4851,7 @@
         <v>318</v>
       </c>
       <c r="M3" s="12" t="s">
-        <v>391</v>
+        <v>438</v>
       </c>
       <c r="Q3" s="12" t="s">
         <v>5</v>
@@ -5000,43 +5000,43 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>413</v>
-      </c>
       <c r="I7" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J7" s="12" t="s">
         <v>3</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L7" s="12" t="s">
         <v>318</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="O7" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="P7"/>
       <c r="Q7" s="12" t="s">
@@ -5051,22 +5051,22 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>204</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>176</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="J8" s="12" t="s">
         <v>3</v>
@@ -5282,7 +5282,7 @@
         <v>7</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>176</v>
@@ -5311,7 +5311,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F15" s="12" t="s">
         <v>176</v>
@@ -5329,7 +5329,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>5</v>
@@ -5632,7 +5632,7 @@
         <v>4</v>
       </c>
       <c r="P24" s="12" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="Q24" s="12" t="s">
         <v>9</v>
@@ -5910,7 +5910,7 @@
         <v>4</v>
       </c>
       <c r="P34" s="12" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="Q34" s="12" t="s">
         <v>9</v>
@@ -5939,7 +5939,7 @@
         <v>4</v>
       </c>
       <c r="M35" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>3</v>
@@ -6053,7 +6053,7 @@
         <v>193</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>214</v>
@@ -6173,37 +6173,37 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>12</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K5" s="12" t="s">
+        <v>416</v>
+      </c>
+      <c r="L5" s="12" t="s">
         <v>417</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>418</v>
       </c>
       <c r="Q5" s="12" t="s">
         <v>5</v>
@@ -6232,19 +6232,19 @@
         <v>75</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I6" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>113</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q6" s="12" t="s">
         <v>5</v>
@@ -6273,7 +6273,7 @@
         <v>8</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I7" s="12" t="s">
         <v>3</v>
@@ -6311,7 +6311,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I8" s="12" t="s">
         <v>3</v>
@@ -6386,10 +6386,10 @@
         <v>4</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>109</v>
@@ -6398,7 +6398,7 @@
         <v>307</v>
       </c>
       <c r="M10" s="12" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Q10" s="12" t="s">
         <v>5</v>
@@ -6502,7 +6502,7 @@
         <v>220</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I13" s="23" t="s">
         <v>3</v>
@@ -6543,7 +6543,7 @@
         <v>199</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>3</v>
@@ -6584,7 +6584,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I15" s="23" t="s">
         <v>3</v>
@@ -6624,7 +6624,7 @@
         <v>286</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>3</v>
@@ -6660,7 +6660,7 @@
       </c>
       <c r="G17" s="26"/>
       <c r="H17" s="12" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I17" s="26" t="s">
         <v>3</v>
@@ -6960,7 +6960,7 @@
         <v>97</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>259</v>
@@ -7177,19 +7177,19 @@
         <v>12</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>327</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q7" s="12" t="s">
         <v>5</v>
@@ -7215,19 +7215,19 @@
         <v>12</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>327</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="Q8" s="12" t="s">
         <v>5</v>
@@ -7375,7 +7375,7 @@
         <v>4</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="Q13" s="12" t="s">
         <v>5</v>
@@ -7442,7 +7442,7 @@
         <v>4</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Q15" s="12" t="s">
         <v>9</v>
@@ -7450,7 +7450,7 @@
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F16" s="12" t="s">
         <v>176</v>
@@ -7468,7 +7468,7 @@
         <v>4</v>
       </c>
       <c r="P16" s="12" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Q16" s="12" t="s">
         <v>5</v>
@@ -7517,10 +7517,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>176</v>
@@ -7538,7 +7538,7 @@
         <v>4</v>
       </c>
       <c r="M18" s="12" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q18" s="12" t="s">
         <v>9</v>
@@ -7654,7 +7654,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="Q22" s="12" t="s">
         <v>9</v>
@@ -7974,7 +7974,7 @@
         <v>4</v>
       </c>
       <c r="P32" s="12" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="Q32" s="12" t="s">
         <v>9</v>
@@ -8070,7 +8070,7 @@
         <v>4</v>
       </c>
       <c r="P35" s="12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="Q35" s="12" t="s">
         <v>9</v>
@@ -8130,7 +8130,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>58</v>
@@ -8148,7 +8148,7 @@
         <v>4</v>
       </c>
       <c r="N38" s="12" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="Q38" s="12" t="s">
         <v>5</v>
@@ -8174,7 +8174,7 @@
         <v>4</v>
       </c>
       <c r="N39" s="12" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="Q39" s="12" t="s">
         <v>5</v>
@@ -8776,7 +8776,7 @@
         <v>375</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="R10" s="16"/>
       <c r="S10" s="16"/>
@@ -8832,7 +8832,7 @@
         <v>4</v>
       </c>
       <c r="P12" s="16" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="Q12" s="2" t="s">
         <v>352</v>

</xml_diff>